<commit_message>
added 'drop' and 'dropExplanation' columns
</commit_message>
<xml_diff>
--- a/myData/LEB 7-19-18 Strain 34 35 36 prelim.xlsx
+++ b/myData/LEB 7-19-18 Strain 34 35 36 prelim.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="123">
   <si>
     <t>A</t>
   </si>
@@ -384,13 +384,19 @@
   </si>
   <si>
     <t>LZ36</t>
+  </si>
+  <si>
+    <t>drop</t>
+  </si>
+  <si>
+    <t>dropExplanation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -432,8 +438,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -512,8 +525,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -547,6 +566,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -573,7 +601,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -624,6 +652,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3144,15 +3179,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" ht="24">
+    <row r="1" spans="1:18" ht="24">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -3201,8 +3236,14 @@
       <c r="P1" s="16" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="9" t="s">
         <v>16</v>
       </c>
@@ -3249,8 +3290,12 @@
       <c r="P2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" s="20"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="9" t="s">
@@ -3287,8 +3332,12 @@
       <c r="P3" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" s="20"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
@@ -3325,8 +3374,12 @@
       <c r="P4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" s="20"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
@@ -3363,8 +3416,12 @@
       <c r="P5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
@@ -3411,8 +3468,12 @@
       <c r="P6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
@@ -3449,8 +3510,12 @@
       <c r="P7">
         <v>40</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" s="20"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
@@ -3487,8 +3552,12 @@
       <c r="P8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -3525,8 +3594,12 @@
       <c r="P9">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" s="20"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
@@ -3573,8 +3646,12 @@
       <c r="P10">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" s="20"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9" t="s">
@@ -3611,8 +3688,12 @@
       <c r="P11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" s="20"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9" t="s">
@@ -3649,8 +3730,12 @@
       <c r="P12">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" s="20"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
@@ -3687,8 +3772,12 @@
       <c r="P13">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" s="20"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
@@ -3735,8 +3824,12 @@
       <c r="P14">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9" t="s">
@@ -3773,8 +3866,12 @@
       <c r="P15">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" s="20"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9" t="s">
@@ -3811,8 +3908,12 @@
       <c r="P16">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" s="20"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
@@ -3849,8 +3950,12 @@
       <c r="P17">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" s="20"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="9" t="s">
         <v>36</v>
       </c>
@@ -3897,8 +4002,12 @@
       <c r="P18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" s="20"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9" t="s">
@@ -3935,8 +4044,12 @@
       <c r="P19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R19" s="20"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9" t="s">
@@ -3973,8 +4086,12 @@
       <c r="P20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R20" s="20"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
@@ -4011,8 +4128,12 @@
       <c r="P21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R21" s="20"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="9" t="s">
         <v>41</v>
       </c>
@@ -4059,8 +4180,12 @@
       <c r="P22">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R22" s="20"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9" t="s">
@@ -4097,8 +4222,12 @@
       <c r="P23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R23" s="20"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9" t="s">
@@ -4135,8 +4264,12 @@
       <c r="P24">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R24" s="20"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
@@ -4173,8 +4306,12 @@
       <c r="P25">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R25" s="20"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="9" t="s">
         <v>46</v>
       </c>
@@ -4221,8 +4358,12 @@
       <c r="P26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R26" s="20"/>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9" t="s">
@@ -4259,8 +4400,12 @@
       <c r="P27">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R27" s="20"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9" t="s">
@@ -4297,8 +4442,12 @@
       <c r="P28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R28" s="20"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9" t="s">
@@ -4335,8 +4484,12 @@
       <c r="P29">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R29" s="20"/>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="9" t="s">
         <v>51</v>
       </c>
@@ -4383,8 +4536,12 @@
       <c r="P30">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R30" s="20"/>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9" t="s">
@@ -4421,8 +4578,12 @@
       <c r="P31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R31" s="20"/>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9" t="s">
@@ -4459,8 +4620,12 @@
       <c r="P32">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R32" s="20"/>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9" t="s">
@@ -4497,8 +4662,12 @@
       <c r="P33">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R33" s="20"/>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="9" t="s">
         <v>56</v>
       </c>
@@ -4545,8 +4714,12 @@
       <c r="P34">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R34" s="20"/>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9" t="s">
@@ -4583,8 +4756,12 @@
       <c r="P35">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R35" s="20"/>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9" t="s">
@@ -4621,8 +4798,12 @@
       <c r="P36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R36" s="20"/>
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9" t="s">
@@ -4659,8 +4840,12 @@
       <c r="P37">
         <v>20</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R37" s="20"/>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="9" t="s">
         <v>61</v>
       </c>
@@ -4707,8 +4892,12 @@
       <c r="P38">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R38" s="20"/>
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9" t="s">
@@ -4745,8 +4934,12 @@
       <c r="P39">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R39" s="20"/>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
@@ -4783,8 +4976,12 @@
       <c r="P40">
         <v>20</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R40" s="20"/>
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9" t="s">
@@ -4821,6 +5018,10 @@
       <c r="P41">
         <v>20</v>
       </c>
+      <c r="Q41" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="R41" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4837,7 +5038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>